<commit_message>
#Ajusté el tema costos.
</commit_message>
<xml_diff>
--- a/meetings/helpers/Costos.20101018.xlsx
+++ b/meetings/helpers/Costos.20101018.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4506"/>
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
     <workbookView xWindow="360" yWindow="300" windowWidth="14880" windowHeight="7815"/>
@@ -9,7 +9,7 @@
   <sheets>
     <sheet name="Cobertura de la Prueba" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="125725"/>
+  <calcPr calcId="124519"/>
 </workbook>
 </file>
 
@@ -164,7 +164,7 @@
 
 <file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <c:lang val="en-US"/>
+  <c:lang val="es-ES_tradnl"/>
   <c:chart>
     <c:autoTitleDeleted val="1"/>
     <c:plotArea>
@@ -219,16 +219,16 @@
                   <c:v>72</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>146</c:v>
+                  <c:v>148</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>220</c:v>
+                  <c:v>222</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>294</c:v>
+                  <c:v>296</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>368</c:v>
+                  <c:v>370</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -282,7 +282,7 @@
                   <c:v>72</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>130</c:v>
+                  <c:v>144</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -336,18 +336,18 @@
                   <c:v>73</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>145</c:v>
+                  <c:v>152</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
         </c:ser>
         <c:marker val="1"/>
-        <c:axId val="92662016"/>
-        <c:axId val="105448192"/>
+        <c:axId val="80152448"/>
+        <c:axId val="80167296"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="92662016"/>
+        <c:axId val="80152448"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -359,7 +359,7 @@
               <a:lstStyle/>
               <a:p>
                 <a:pPr>
-                  <a:defRPr/>
+                  <a:defRPr lang="en-US"/>
                 </a:pPr>
                 <a:r>
                   <a:rPr lang="en-US"/>
@@ -373,14 +373,24 @@
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="105448192"/>
+        <c:txPr>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr lang="en-US"/>
+            </a:pPr>
+            <a:endParaRPr lang="es-ES_tradnl"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="80167296"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="105448192"/>
+        <c:axId val="80167296"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -393,7 +403,7 @@
               <a:lstStyle/>
               <a:p>
                 <a:pPr>
-                  <a:defRPr/>
+                  <a:defRPr lang="en-US"/>
                 </a:pPr>
                 <a:r>
                   <a:rPr lang="en-US"/>
@@ -407,7 +417,17 @@
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="92662016"/>
+        <c:txPr>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr lang="en-US"/>
+            </a:pPr>
+            <a:endParaRPr lang="es-ES_tradnl"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="80152448"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -415,17 +435,37 @@
         <c:showHorzBorder val="1"/>
         <c:showVertBorder val="1"/>
         <c:showOutline val="1"/>
+        <c:txPr>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr rtl="0">
+              <a:defRPr lang="en-US"/>
+            </a:pPr>
+            <a:endParaRPr lang="es-ES_tradnl"/>
+          </a:p>
+        </c:txPr>
       </c:dTable>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
       <c:layout/>
+      <c:txPr>
+        <a:bodyPr/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr lang="en-US"/>
+          </a:pPr>
+          <a:endParaRPr lang="es-ES_tradnl"/>
+        </a:p>
+      </c:txPr>
     </c:legend>
     <c:plotVisOnly val="1"/>
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000133" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000133" header="0.30000000000000032" footer="0.30000000000000032"/>
+    <c:pageMargins b="0.75000000000000144" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000144" header="0.30000000000000032" footer="0.30000000000000032"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -769,7 +809,7 @@
   <dimension ref="A1:D7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C5" sqref="C5"/>
+      <selection activeCell="D4" sqref="D4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
@@ -821,14 +861,14 @@
         <v>2</v>
       </c>
       <c r="B4" s="3">
-        <f>B3+74</f>
-        <v>146</v>
+        <f>B3+76</f>
+        <v>148</v>
       </c>
       <c r="C4" s="3">
-        <v>130</v>
+        <v>144</v>
       </c>
       <c r="D4" s="3">
-        <v>145</v>
+        <v>152</v>
       </c>
     </row>
     <row r="5" spans="1:4">
@@ -837,7 +877,7 @@
       </c>
       <c r="B5" s="3">
         <f>B4+74</f>
-        <v>220</v>
+        <v>222</v>
       </c>
       <c r="C5" s="3"/>
       <c r="D5" s="3"/>
@@ -848,7 +888,7 @@
       </c>
       <c r="B6" s="3">
         <f>B5+74</f>
-        <v>294</v>
+        <v>296</v>
       </c>
       <c r="C6" s="3"/>
       <c r="D6" s="3"/>
@@ -859,7 +899,7 @@
       </c>
       <c r="B7" s="3">
         <f>B6+74</f>
-        <v>368</v>
+        <v>370</v>
       </c>
       <c r="C7" s="3"/>
       <c r="D7" s="3"/>

</xml_diff>